<commit_message>
2018-06-29 use openpyxl write xlsx
Signed-off-by: 舒露 <shulubanggood>
</commit_message>
<xml_diff>
--- a/demomd/pipelines.xlsx
+++ b/demomd/pipelines.xlsx
@@ -4,18 +4,18 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12780" windowWidth="27480"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>pipeline_id</t>
   </si>
@@ -26,44 +26,415 @@
     <t>author_email</t>
   </si>
   <si>
+    <t>branch</t>
+  </si>
+  <si>
     <t>commit_id</t>
   </si>
   <si>
     <t>commit_message</t>
   </si>
   <si>
-    <t>branch</t>
-  </si>
-  <si>
     <t>pipeline_status</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+  <numFmts count="4">
+    <numFmt formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ " numFmtId="164"/>
+    <numFmt formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ " numFmtId="165"/>
+    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="166"/>
+    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="167"/>
+  </numFmts>
+  <fonts count="23">
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+      <color rgb="FF000000"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
       <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -72,24 +443,313 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="14" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="167">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="6" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="10" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="10" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="18" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="27" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="49">
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="7" name="货币[0]" xfId="1"/>
+    <cellStyle builtinId="38" name="20% - 强调文字颜色 3" xfId="2"/>
+    <cellStyle builtinId="20" name="输入" xfId="3"/>
+    <cellStyle builtinId="4" name="货币" xfId="4"/>
+    <cellStyle builtinId="6" name="千位分隔[0]" xfId="5"/>
+    <cellStyle builtinId="39" name="40% - 强调文字颜色 3" xfId="6"/>
+    <cellStyle builtinId="27" name="差" xfId="7"/>
+    <cellStyle builtinId="3" name="千位分隔" xfId="8"/>
+    <cellStyle builtinId="40" name="60% - 强调文字颜色 3" xfId="9"/>
+    <cellStyle builtinId="8" name="超链接" xfId="10"/>
+    <cellStyle builtinId="5" name="百分比" xfId="11"/>
+    <cellStyle builtinId="9" name="已访问的超链接" xfId="12"/>
+    <cellStyle builtinId="10" name="注释" xfId="13"/>
+    <cellStyle builtinId="36" name="60% - 强调文字颜色 2" xfId="14"/>
+    <cellStyle builtinId="19" name="标题 4" xfId="15"/>
+    <cellStyle builtinId="11" name="警告文本" xfId="16"/>
+    <cellStyle builtinId="15" name="标题" xfId="17"/>
+    <cellStyle builtinId="53" name="解释性文本" xfId="18"/>
+    <cellStyle builtinId="16" name="标题 1" xfId="19"/>
+    <cellStyle builtinId="17" name="标题 2" xfId="20"/>
+    <cellStyle builtinId="32" name="60% - 强调文字颜色 1" xfId="21"/>
+    <cellStyle builtinId="18" name="标题 3" xfId="22"/>
+    <cellStyle builtinId="44" name="60% - 强调文字颜色 4" xfId="23"/>
+    <cellStyle builtinId="21" name="输出" xfId="24"/>
+    <cellStyle builtinId="22" name="计算" xfId="25"/>
+    <cellStyle builtinId="23" name="检查单元格" xfId="26"/>
+    <cellStyle builtinId="50" name="20% - 强调文字颜色 6" xfId="27"/>
+    <cellStyle builtinId="33" name="强调文字颜色 2" xfId="28"/>
+    <cellStyle builtinId="24" name="链接单元格" xfId="29"/>
+    <cellStyle builtinId="25" name="汇总" xfId="30"/>
+    <cellStyle builtinId="26" name="好" xfId="31"/>
+    <cellStyle builtinId="28" name="适中" xfId="32"/>
+    <cellStyle builtinId="46" name="20% - 强调文字颜色 5" xfId="33"/>
+    <cellStyle builtinId="29" name="强调文字颜色 1" xfId="34"/>
+    <cellStyle builtinId="30" name="20% - 强调文字颜色 1" xfId="35"/>
+    <cellStyle builtinId="31" name="40% - 强调文字颜色 1" xfId="36"/>
+    <cellStyle builtinId="34" name="20% - 强调文字颜色 2" xfId="37"/>
+    <cellStyle builtinId="35" name="40% - 强调文字颜色 2" xfId="38"/>
+    <cellStyle builtinId="37" name="强调文字颜色 3" xfId="39"/>
+    <cellStyle builtinId="41" name="强调文字颜色 4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - 强调文字颜色 4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - 强调文字颜色 4" xfId="42"/>
+    <cellStyle builtinId="45" name="强调文字颜色 5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - 强调文字颜色 5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - 强调文字颜色 5" xfId="45"/>
+    <cellStyle builtinId="49" name="强调文字颜色 6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - 强调文字颜色 6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - 强调文字颜色 6" xfId="48"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -374,7 +1034,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -384,61 +1043,68 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14.5"/>
+    <col customWidth="1" max="2" min="2" width="18.375"/>
+    <col customWidth="1" max="4" min="3" width="22.25"/>
+    <col customWidth="1" max="5" min="5" width="21.75"/>
+    <col customWidth="1" max="6" min="6" width="22"/>
+    <col customWidth="1" max="8" min="7" width="21.25"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" s="1" t="s">
+    <row customFormat="1" customHeight="1" ht="21" r="1" s="1" spans="1:9">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="n"/>
+      <c r="I1" s="3" t="n"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>